<commit_message>
continuation of the work
</commit_message>
<xml_diff>
--- a/Meteo Only/median_Q1_Q3.xlsx
+++ b/Meteo Only/median_Q1_Q3.xlsx
@@ -468,13 +468,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>3.200000047683716</v>
+        <v>3.099999904632568</v>
       </c>
       <c r="D2" t="n">
-        <v>3.200000047683716</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E2" t="n">
-        <v>3.200000047683716</v>
+        <v>3.799999952316284</v>
       </c>
     </row>
     <row r="3">
@@ -488,10 +488,10 @@
         <v>3.200000047683716</v>
       </c>
       <c r="D3" t="n">
-        <v>3.200000047683716</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E3" t="n">
-        <v>3.200000047683716</v>
+        <v>3.700000047683716</v>
       </c>
     </row>
     <row r="4">
@@ -502,13 +502,13 @@
         <v>20</v>
       </c>
       <c r="C4" t="n">
-        <v>3.200000047683716</v>
+        <v>3.099999904632568</v>
       </c>
       <c r="D4" t="n">
-        <v>3.200000047683716</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E4" t="n">
-        <v>3.200000047683716</v>
+        <v>3.700000047683716</v>
       </c>
     </row>
     <row r="5">
@@ -519,13 +519,13 @@
         <v>30</v>
       </c>
       <c r="C5" t="n">
-        <v>3.200000047683716</v>
+        <v>3.099999904632568</v>
       </c>
       <c r="D5" t="n">
-        <v>3.200000047683716</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E5" t="n">
-        <v>3.200000047683716</v>
+        <v>3.700000047683716</v>
       </c>
     </row>
     <row r="6">
@@ -536,13 +536,13 @@
         <v>40</v>
       </c>
       <c r="C6" t="n">
-        <v>3.200000047683716</v>
+        <v>3.099999904632568</v>
       </c>
       <c r="D6" t="n">
-        <v>3.200000047683716</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E6" t="n">
-        <v>3.200000047683716</v>
+        <v>3.700000047683716</v>
       </c>
     </row>
     <row r="7">
@@ -553,13 +553,13 @@
         <v>50</v>
       </c>
       <c r="C7" t="n">
-        <v>3.200000047683716</v>
+        <v>3.099999904632568</v>
       </c>
       <c r="D7" t="n">
-        <v>3.200000047683716</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E7" t="n">
-        <v>3.200000047683716</v>
+        <v>3.700000047683716</v>
       </c>
     </row>
     <row r="8">
@@ -570,13 +570,13 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>3.200000047683716</v>
+        <v>3.099999904632568</v>
       </c>
       <c r="D8" t="n">
-        <v>3.200000047683716</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E8" t="n">
-        <v>3.200000047683716</v>
+        <v>3.700000047683716</v>
       </c>
     </row>
     <row r="9">
@@ -587,13 +587,13 @@
         <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>3.200000047683716</v>
+        <v>3.099999904632568</v>
       </c>
       <c r="D9" t="n">
-        <v>3.200000047683716</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E9" t="n">
-        <v>3.200000047683716</v>
+        <v>3.700000047683716</v>
       </c>
     </row>
     <row r="10">
@@ -604,13 +604,13 @@
         <v>20</v>
       </c>
       <c r="C10" t="n">
-        <v>3.200000047683716</v>
+        <v>3.099999904632568</v>
       </c>
       <c r="D10" t="n">
-        <v>3.200000047683716</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E10" t="n">
-        <v>3.200000047683716</v>
+        <v>3.700000047683716</v>
       </c>
     </row>
     <row r="11">
@@ -621,13 +621,13 @@
         <v>30</v>
       </c>
       <c r="C11" t="n">
-        <v>3.150000095367432</v>
+        <v>3.099999904632568</v>
       </c>
       <c r="D11" t="n">
-        <v>3.149999976158142</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E11" t="n">
-        <v>3.149999976158142</v>
+        <v>3.700000047683716</v>
       </c>
     </row>
     <row r="12">
@@ -641,10 +641,10 @@
         <v>3.099999904632568</v>
       </c>
       <c r="D12" t="n">
-        <v>3.099999904632568</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E12" t="n">
-        <v>3.099999904632568</v>
+        <v>3.599999904632568</v>
       </c>
     </row>
     <row r="13">
@@ -658,10 +658,10 @@
         <v>3.099999904632568</v>
       </c>
       <c r="D13" t="n">
-        <v>3.099999904632568</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E13" t="n">
-        <v>3.099999904632568</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="14">
@@ -672,13 +672,13 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>3.200000047683716</v>
+        <v>3.099999904632568</v>
       </c>
       <c r="D14" t="n">
-        <v>3.200000047683716</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E14" t="n">
-        <v>3.200000047683716</v>
+        <v>3.599999904632568</v>
       </c>
     </row>
     <row r="15">
@@ -689,13 +689,13 @@
         <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>3.200000047683716</v>
+        <v>3.099999904632568</v>
       </c>
       <c r="D15" t="n">
-        <v>3.200000047683716</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E15" t="n">
-        <v>3.200000047683716</v>
+        <v>3.599999904632568</v>
       </c>
     </row>
     <row r="16">
@@ -709,10 +709,10 @@
         <v>3.099999904632568</v>
       </c>
       <c r="D16" t="n">
-        <v>3.099999904632568</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E16" t="n">
-        <v>3.099999904632568</v>
+        <v>3.549999952316284</v>
       </c>
     </row>
     <row r="17">
@@ -726,10 +726,10 @@
         <v>3.099999904632568</v>
       </c>
       <c r="D17" t="n">
-        <v>3.099999904632568</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E17" t="n">
-        <v>3.099999904632568</v>
+        <v>3.549999952316284</v>
       </c>
     </row>
     <row r="18">
@@ -740,13 +740,13 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>3.150000095367432</v>
+        <v>3.099999904632568</v>
       </c>
       <c r="D18" t="n">
-        <v>3.149999976158142</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E18" t="n">
-        <v>3.149999976158142</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="19">
@@ -760,10 +760,10 @@
         <v>3.099999904632568</v>
       </c>
       <c r="D19" t="n">
-        <v>3.099999904632568</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E19" t="n">
-        <v>3.099999904632568</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="20">
@@ -777,10 +777,10 @@
         <v>3.099999904632568</v>
       </c>
       <c r="D20" t="n">
-        <v>3.099999904632568</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E20" t="n">
-        <v>3.099999904632568</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="21">
@@ -794,10 +794,10 @@
         <v>3.099999904632568</v>
       </c>
       <c r="D21" t="n">
-        <v>3.099999904632568</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E21" t="n">
-        <v>3.099999904632568</v>
+        <v>3.549999952316284</v>
       </c>
     </row>
     <row r="22">
@@ -811,10 +811,10 @@
         <v>3.099999904632568</v>
       </c>
       <c r="D22" t="n">
-        <v>3.099999904632568</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E22" t="n">
-        <v>3.099999904632568</v>
+        <v>3.599999904632568</v>
       </c>
     </row>
     <row r="23">
@@ -828,10 +828,10 @@
         <v>3.099999904632568</v>
       </c>
       <c r="D23" t="n">
-        <v>3.099999904632568</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E23" t="n">
-        <v>3.099999904632568</v>
+        <v>3.900000095367432</v>
       </c>
     </row>
     <row r="24">
@@ -845,10 +845,10 @@
         <v>3.099999904632568</v>
       </c>
       <c r="D24" t="n">
-        <v>3.099999904632568</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E24" t="n">
-        <v>3.099999904632568</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
@@ -862,10 +862,10 @@
         <v>3.099999904632568</v>
       </c>
       <c r="D25" t="n">
-        <v>3.099999904632568</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E25" t="n">
-        <v>3.099999904632568</v>
+        <v>4.300000190734863</v>
       </c>
     </row>
     <row r="26">
@@ -879,10 +879,10 @@
         <v>3.099999904632568</v>
       </c>
       <c r="D26" t="n">
-        <v>3.099999904632568</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E26" t="n">
-        <v>3.099999904632568</v>
+        <v>4.950000047683716</v>
       </c>
     </row>
     <row r="27">
@@ -896,10 +896,10 @@
         <v>3.099999904632568</v>
       </c>
       <c r="D27" t="n">
-        <v>3.099999904632568</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="E27" t="n">
-        <v>3.099999904632568</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28">
@@ -913,10 +913,10 @@
         <v>3.099999904632568</v>
       </c>
       <c r="D28" t="n">
-        <v>3.099999904632568</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E28" t="n">
-        <v>3.099999904632568</v>
+        <v>9.924999952316284</v>
       </c>
     </row>
     <row r="29">
@@ -930,10 +930,10 @@
         <v>3.099999904632568</v>
       </c>
       <c r="D29" t="n">
-        <v>3.099999904632568</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E29" t="n">
-        <v>3.099999904632568</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30">
@@ -944,13 +944,13 @@
         <v>40</v>
       </c>
       <c r="C30" t="n">
-        <v>3.099999904632568</v>
+        <v>3.200000047683716</v>
       </c>
       <c r="D30" t="n">
-        <v>3.099999904632568</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E30" t="n">
-        <v>3.099999904632568</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31">
@@ -961,13 +961,13 @@
         <v>50</v>
       </c>
       <c r="C31" t="n">
-        <v>3.099999904632568</v>
+        <v>3.299999952316284</v>
       </c>
       <c r="D31" t="n">
-        <v>3.099999904632568</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E31" t="n">
-        <v>3.099999904632568</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32">
@@ -978,13 +978,13 @@
         <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>3.099999904632568</v>
+        <v>3.5</v>
       </c>
       <c r="D32" t="n">
-        <v>3.099999904632568</v>
+        <v>2.799999952316284</v>
       </c>
       <c r="E32" t="n">
-        <v>3.099999904632568</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33">
@@ -995,13 +995,13 @@
         <v>10</v>
       </c>
       <c r="C33" t="n">
-        <v>3.099999904632568</v>
+        <v>4.800000190734863</v>
       </c>
       <c r="D33" t="n">
-        <v>3.099999904632568</v>
+        <v>2.799999952316284</v>
       </c>
       <c r="E33" t="n">
-        <v>3.099999904632568</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34">
@@ -1012,13 +1012,13 @@
         <v>20</v>
       </c>
       <c r="C34" t="n">
-        <v>3.099999904632568</v>
+        <v>6.199999809265137</v>
       </c>
       <c r="D34" t="n">
-        <v>3.099999904632568</v>
+        <v>2.799999952316284</v>
       </c>
       <c r="E34" t="n">
-        <v>3.099999904632568</v>
+        <v>78.5</v>
       </c>
     </row>
     <row r="35">
@@ -1029,13 +1029,13 @@
         <v>30</v>
       </c>
       <c r="C35" t="n">
-        <v>3.099999904632568</v>
+        <v>9.899999618530273</v>
       </c>
       <c r="D35" t="n">
-        <v>3.099999904632568</v>
+        <v>2.900000095367432</v>
       </c>
       <c r="E35" t="n">
-        <v>3.099999904632568</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="36">
@@ -1046,13 +1046,13 @@
         <v>40</v>
       </c>
       <c r="C36" t="n">
-        <v>3.099999904632568</v>
+        <v>15</v>
       </c>
       <c r="D36" t="n">
-        <v>3.099999904632568</v>
+        <v>3</v>
       </c>
       <c r="E36" t="n">
-        <v>3.099999904632568</v>
+        <v>113.5</v>
       </c>
     </row>
     <row r="37">
@@ -1063,13 +1063,13 @@
         <v>50</v>
       </c>
       <c r="C37" t="n">
-        <v>3.099999904632568</v>
+        <v>21</v>
       </c>
       <c r="D37" t="n">
-        <v>3.099999904632568</v>
+        <v>3.350000023841858</v>
       </c>
       <c r="E37" t="n">
-        <v>3.099999904632568</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38">
@@ -1080,13 +1080,13 @@
         <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>3.099999904632568</v>
+        <v>30</v>
       </c>
       <c r="D38" t="n">
-        <v>3.099999904632568</v>
+        <v>4.699999809265137</v>
       </c>
       <c r="E38" t="n">
-        <v>3.099999904632568</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39">
@@ -1097,13 +1097,13 @@
         <v>10</v>
       </c>
       <c r="C39" t="n">
-        <v>3.099999904632568</v>
+        <v>45</v>
       </c>
       <c r="D39" t="n">
-        <v>3.099999904632568</v>
+        <v>6.549999952316284</v>
       </c>
       <c r="E39" t="n">
-        <v>3.099999904632568</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40">
@@ -1114,13 +1114,13 @@
         <v>20</v>
       </c>
       <c r="C40" t="n">
-        <v>3.099999904632568</v>
+        <v>58</v>
       </c>
       <c r="D40" t="n">
-        <v>3.099999904632568</v>
+        <v>9.75</v>
       </c>
       <c r="E40" t="n">
-        <v>3.099999904632568</v>
+        <v>198.5</v>
       </c>
     </row>
     <row r="41">
@@ -1131,13 +1131,13 @@
         <v>30</v>
       </c>
       <c r="C41" t="n">
-        <v>3.099999904632568</v>
+        <v>60</v>
       </c>
       <c r="D41" t="n">
-        <v>3.099999904632568</v>
+        <v>16</v>
       </c>
       <c r="E41" t="n">
-        <v>3.099999904632568</v>
+        <v>177.5</v>
       </c>
     </row>
     <row r="42">
@@ -1148,13 +1148,13 @@
         <v>40</v>
       </c>
       <c r="C42" t="n">
-        <v>3.200000047683716</v>
+        <v>74</v>
       </c>
       <c r="D42" t="n">
-        <v>3.200000047683716</v>
+        <v>21.5</v>
       </c>
       <c r="E42" t="n">
-        <v>3.200000047683716</v>
+        <v>209.5</v>
       </c>
     </row>
     <row r="43">
@@ -1165,13 +1165,13 @@
         <v>50</v>
       </c>
       <c r="C43" t="n">
-        <v>3.299999952316284</v>
+        <v>99</v>
       </c>
       <c r="D43" t="n">
-        <v>3.299999952316284</v>
+        <v>29</v>
       </c>
       <c r="E43" t="n">
-        <v>3.299999952316284</v>
+        <v>247</v>
       </c>
     </row>
     <row r="44">
@@ -1182,13 +1182,13 @@
         <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>3.5</v>
+        <v>122</v>
       </c>
       <c r="D44" t="n">
-        <v>3.5</v>
+        <v>35.5</v>
       </c>
       <c r="E44" t="n">
-        <v>3.5</v>
+        <v>257</v>
       </c>
     </row>
     <row r="45">
@@ -1199,13 +1199,13 @@
         <v>10</v>
       </c>
       <c r="C45" t="n">
-        <v>4.800000190734863</v>
+        <v>140</v>
       </c>
       <c r="D45" t="n">
-        <v>4.800000190734863</v>
+        <v>47</v>
       </c>
       <c r="E45" t="n">
-        <v>4.800000190734863</v>
+        <v>306.5</v>
       </c>
     </row>
     <row r="46">
@@ -1216,13 +1216,13 @@
         <v>20</v>
       </c>
       <c r="C46" t="n">
-        <v>6.199999809265137</v>
+        <v>154</v>
       </c>
       <c r="D46" t="n">
-        <v>6.199999809265137</v>
+        <v>58.5</v>
       </c>
       <c r="E46" t="n">
-        <v>6.199999809265137</v>
+        <v>328</v>
       </c>
     </row>
     <row r="47">
@@ -1233,13 +1233,13 @@
         <v>30</v>
       </c>
       <c r="C47" t="n">
-        <v>9.899999618530273</v>
+        <v>174</v>
       </c>
       <c r="D47" t="n">
-        <v>9.899999618530273</v>
+        <v>67</v>
       </c>
       <c r="E47" t="n">
-        <v>9.899999618530273</v>
+        <v>357</v>
       </c>
     </row>
     <row r="48">
@@ -1250,13 +1250,13 @@
         <v>40</v>
       </c>
       <c r="C48" t="n">
-        <v>15</v>
+        <v>192</v>
       </c>
       <c r="D48" t="n">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="E48" t="n">
-        <v>15</v>
+        <v>405</v>
       </c>
     </row>
     <row r="49">
@@ -1267,13 +1267,13 @@
         <v>50</v>
       </c>
       <c r="C49" t="n">
-        <v>21</v>
+        <v>211</v>
       </c>
       <c r="D49" t="n">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="E49" t="n">
-        <v>21</v>
+        <v>430</v>
       </c>
     </row>
     <row r="50">
@@ -1284,13 +1284,13 @@
         <v>0</v>
       </c>
       <c r="C50" t="n">
-        <v>30</v>
+        <v>230</v>
       </c>
       <c r="D50" t="n">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="E50" t="n">
-        <v>30</v>
+        <v>448</v>
       </c>
     </row>
     <row r="51">
@@ -1301,13 +1301,13 @@
         <v>10</v>
       </c>
       <c r="C51" t="n">
-        <v>45</v>
+        <v>250</v>
       </c>
       <c r="D51" t="n">
-        <v>45</v>
+        <v>99.5</v>
       </c>
       <c r="E51" t="n">
-        <v>45</v>
+        <v>480</v>
       </c>
     </row>
     <row r="52">
@@ -1318,13 +1318,13 @@
         <v>20</v>
       </c>
       <c r="C52" t="n">
-        <v>58</v>
+        <v>254</v>
       </c>
       <c r="D52" t="n">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="E52" t="n">
-        <v>58</v>
+        <v>518.5</v>
       </c>
     </row>
     <row r="53">
@@ -1335,13 +1335,13 @@
         <v>30</v>
       </c>
       <c r="C53" t="n">
-        <v>60</v>
+        <v>273</v>
       </c>
       <c r="D53" t="n">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="E53" t="n">
-        <v>60</v>
+        <v>533.5</v>
       </c>
     </row>
     <row r="54">
@@ -1352,13 +1352,13 @@
         <v>40</v>
       </c>
       <c r="C54" t="n">
-        <v>74</v>
+        <v>292</v>
       </c>
       <c r="D54" t="n">
-        <v>74</v>
+        <v>124</v>
       </c>
       <c r="E54" t="n">
-        <v>74</v>
+        <v>561.5</v>
       </c>
     </row>
     <row r="55">
@@ -1369,13 +1369,13 @@
         <v>50</v>
       </c>
       <c r="C55" t="n">
-        <v>99</v>
+        <v>315</v>
       </c>
       <c r="D55" t="n">
-        <v>99</v>
+        <v>143</v>
       </c>
       <c r="E55" t="n">
-        <v>99</v>
+        <v>577</v>
       </c>
     </row>
     <row r="56">
@@ -1386,13 +1386,13 @@
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>122</v>
+        <v>325</v>
       </c>
       <c r="D56" t="n">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="E56" t="n">
-        <v>122</v>
+        <v>586</v>
       </c>
     </row>
     <row r="57">
@@ -1403,13 +1403,13 @@
         <v>10</v>
       </c>
       <c r="C57" t="n">
-        <v>140</v>
+        <v>345</v>
       </c>
       <c r="D57" t="n">
-        <v>140</v>
+        <v>159.5</v>
       </c>
       <c r="E57" t="n">
-        <v>140</v>
+        <v>602</v>
       </c>
     </row>
     <row r="58">
@@ -1420,13 +1420,13 @@
         <v>20</v>
       </c>
       <c r="C58" t="n">
-        <v>154</v>
+        <v>347</v>
       </c>
       <c r="D58" t="n">
-        <v>154</v>
+        <v>167.5</v>
       </c>
       <c r="E58" t="n">
-        <v>154</v>
+        <v>617</v>
       </c>
     </row>
     <row r="59">
@@ -1437,13 +1437,13 @@
         <v>30</v>
       </c>
       <c r="C59" t="n">
-        <v>174</v>
+        <v>350</v>
       </c>
       <c r="D59" t="n">
-        <v>174</v>
+        <v>175.5</v>
       </c>
       <c r="E59" t="n">
-        <v>174</v>
+        <v>601</v>
       </c>
     </row>
     <row r="60">
@@ -1454,13 +1454,13 @@
         <v>40</v>
       </c>
       <c r="C60" t="n">
-        <v>192</v>
+        <v>359</v>
       </c>
       <c r="D60" t="n">
-        <v>192</v>
+        <v>183.5</v>
       </c>
       <c r="E60" t="n">
-        <v>192</v>
+        <v>636</v>
       </c>
     </row>
     <row r="61">
@@ -1471,13 +1471,13 @@
         <v>50</v>
       </c>
       <c r="C61" t="n">
-        <v>211</v>
+        <v>375</v>
       </c>
       <c r="D61" t="n">
-        <v>211</v>
+        <v>185</v>
       </c>
       <c r="E61" t="n">
-        <v>211</v>
+        <v>653</v>
       </c>
     </row>
     <row r="62">
@@ -1488,13 +1488,13 @@
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>230</v>
+        <v>405</v>
       </c>
       <c r="D62" t="n">
-        <v>230</v>
+        <v>181.5</v>
       </c>
       <c r="E62" t="n">
-        <v>230</v>
+        <v>694.5</v>
       </c>
     </row>
     <row r="63">
@@ -1505,13 +1505,13 @@
         <v>10</v>
       </c>
       <c r="C63" t="n">
-        <v>250</v>
+        <v>402</v>
       </c>
       <c r="D63" t="n">
-        <v>250</v>
+        <v>180</v>
       </c>
       <c r="E63" t="n">
-        <v>250</v>
+        <v>683.5</v>
       </c>
     </row>
     <row r="64">
@@ -1522,13 +1522,13 @@
         <v>20</v>
       </c>
       <c r="C64" t="n">
-        <v>254</v>
+        <v>406</v>
       </c>
       <c r="D64" t="n">
-        <v>254</v>
+        <v>195.5</v>
       </c>
       <c r="E64" t="n">
-        <v>254</v>
+        <v>691.75</v>
       </c>
     </row>
     <row r="65">
@@ -1539,13 +1539,13 @@
         <v>30</v>
       </c>
       <c r="C65" t="n">
-        <v>273</v>
+        <v>412</v>
       </c>
       <c r="D65" t="n">
-        <v>273</v>
+        <v>194.5</v>
       </c>
       <c r="E65" t="n">
-        <v>273</v>
+        <v>700</v>
       </c>
     </row>
     <row r="66">
@@ -1556,13 +1556,13 @@
         <v>40</v>
       </c>
       <c r="C66" t="n">
-        <v>292</v>
+        <v>417</v>
       </c>
       <c r="D66" t="n">
-        <v>292</v>
+        <v>193.5</v>
       </c>
       <c r="E66" t="n">
-        <v>292</v>
+        <v>702.5</v>
       </c>
     </row>
     <row r="67">
@@ -1573,13 +1573,13 @@
         <v>50</v>
       </c>
       <c r="C67" t="n">
-        <v>315</v>
+        <v>414</v>
       </c>
       <c r="D67" t="n">
-        <v>315</v>
+        <v>199</v>
       </c>
       <c r="E67" t="n">
-        <v>315</v>
+        <v>714</v>
       </c>
     </row>
     <row r="68">
@@ -1590,13 +1590,13 @@
         <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>325</v>
+        <v>420</v>
       </c>
       <c r="D68" t="n">
-        <v>325</v>
+        <v>202</v>
       </c>
       <c r="E68" t="n">
-        <v>325</v>
+        <v>721.5</v>
       </c>
     </row>
     <row r="69">
@@ -1607,13 +1607,13 @@
         <v>10</v>
       </c>
       <c r="C69" t="n">
-        <v>345</v>
+        <v>441</v>
       </c>
       <c r="D69" t="n">
-        <v>345</v>
+        <v>205.5</v>
       </c>
       <c r="E69" t="n">
-        <v>345</v>
+        <v>734</v>
       </c>
     </row>
     <row r="70">
@@ -1624,13 +1624,13 @@
         <v>20</v>
       </c>
       <c r="C70" t="n">
-        <v>348.5</v>
+        <v>421.5</v>
       </c>
       <c r="D70" t="n">
-        <v>348.5</v>
+        <v>200.25</v>
       </c>
       <c r="E70" t="n">
-        <v>348.5</v>
+        <v>716</v>
       </c>
     </row>
     <row r="71">
@@ -1641,13 +1641,13 @@
         <v>30</v>
       </c>
       <c r="C71" t="n">
-        <v>350</v>
+        <v>441</v>
       </c>
       <c r="D71" t="n">
-        <v>350</v>
+        <v>202.5</v>
       </c>
       <c r="E71" t="n">
-        <v>350</v>
+        <v>769.25</v>
       </c>
     </row>
     <row r="72">
@@ -1658,13 +1658,13 @@
         <v>40</v>
       </c>
       <c r="C72" t="n">
-        <v>360</v>
+        <v>439</v>
       </c>
       <c r="D72" t="n">
-        <v>360</v>
+        <v>184</v>
       </c>
       <c r="E72" t="n">
-        <v>360</v>
+        <v>734.25</v>
       </c>
     </row>
     <row r="73">
@@ -1675,13 +1675,13 @@
         <v>50</v>
       </c>
       <c r="C73" t="n">
-        <v>375</v>
+        <v>422.5</v>
       </c>
       <c r="D73" t="n">
-        <v>375</v>
+        <v>180.25</v>
       </c>
       <c r="E73" t="n">
-        <v>375</v>
+        <v>738.75</v>
       </c>
     </row>
     <row r="74">
@@ -1695,10 +1695,10 @@
         <v>405</v>
       </c>
       <c r="D74" t="n">
-        <v>405</v>
+        <v>164.75</v>
       </c>
       <c r="E74" t="n">
-        <v>405</v>
+        <v>722</v>
       </c>
     </row>
     <row r="75">
@@ -1709,13 +1709,13 @@
         <v>10</v>
       </c>
       <c r="C75" t="n">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D75" t="n">
-        <v>403</v>
+        <v>160.75</v>
       </c>
       <c r="E75" t="n">
-        <v>403</v>
+        <v>717.5</v>
       </c>
     </row>
     <row r="76">
@@ -1726,13 +1726,13 @@
         <v>20</v>
       </c>
       <c r="C76" t="n">
-        <v>408.5</v>
+        <v>376</v>
       </c>
       <c r="D76" t="n">
-        <v>408.5</v>
+        <v>157.25</v>
       </c>
       <c r="E76" t="n">
-        <v>408.5</v>
+        <v>711.5</v>
       </c>
     </row>
     <row r="77">
@@ -1743,13 +1743,13 @@
         <v>30</v>
       </c>
       <c r="C77" t="n">
-        <v>412</v>
+        <v>370</v>
       </c>
       <c r="D77" t="n">
-        <v>412</v>
+        <v>158</v>
       </c>
       <c r="E77" t="n">
-        <v>412</v>
+        <v>714.5</v>
       </c>
     </row>
     <row r="78">
@@ -1760,13 +1760,13 @@
         <v>40</v>
       </c>
       <c r="C78" t="n">
-        <v>419.5</v>
+        <v>361.5</v>
       </c>
       <c r="D78" t="n">
-        <v>419.5</v>
+        <v>155.25</v>
       </c>
       <c r="E78" t="n">
-        <v>419.5</v>
+        <v>693.25</v>
       </c>
     </row>
     <row r="79">
@@ -1777,13 +1777,13 @@
         <v>50</v>
       </c>
       <c r="C79" t="n">
-        <v>419</v>
+        <v>344.5</v>
       </c>
       <c r="D79" t="n">
-        <v>419</v>
+        <v>145.5</v>
       </c>
       <c r="E79" t="n">
-        <v>419</v>
+        <v>677.25</v>
       </c>
     </row>
     <row r="80">
@@ -1794,13 +1794,13 @@
         <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>423</v>
+        <v>325.5</v>
       </c>
       <c r="D80" t="n">
-        <v>423</v>
+        <v>139</v>
       </c>
       <c r="E80" t="n">
-        <v>423</v>
+        <v>671</v>
       </c>
     </row>
     <row r="81">
@@ -1811,13 +1811,13 @@
         <v>10</v>
       </c>
       <c r="C81" t="n">
-        <v>441</v>
+        <v>312.5</v>
       </c>
       <c r="D81" t="n">
-        <v>441</v>
+        <v>132.75</v>
       </c>
       <c r="E81" t="n">
-        <v>441</v>
+        <v>657.5</v>
       </c>
     </row>
     <row r="82">
@@ -1828,13 +1828,13 @@
         <v>20</v>
       </c>
       <c r="C82" t="n">
-        <v>421.5</v>
+        <v>287</v>
       </c>
       <c r="D82" t="n">
-        <v>421.5</v>
+        <v>127</v>
       </c>
       <c r="E82" t="n">
-        <v>421.5</v>
+        <v>648.5</v>
       </c>
     </row>
     <row r="83">
@@ -1845,13 +1845,13 @@
         <v>30</v>
       </c>
       <c r="C83" t="n">
-        <v>441</v>
+        <v>274</v>
       </c>
       <c r="D83" t="n">
-        <v>441</v>
+        <v>104.75</v>
       </c>
       <c r="E83" t="n">
-        <v>441</v>
+        <v>625.25</v>
       </c>
     </row>
     <row r="84">
@@ -1862,13 +1862,13 @@
         <v>40</v>
       </c>
       <c r="C84" t="n">
-        <v>439</v>
+        <v>255.5</v>
       </c>
       <c r="D84" t="n">
-        <v>439</v>
+        <v>89</v>
       </c>
       <c r="E84" t="n">
-        <v>439</v>
+        <v>599.25</v>
       </c>
     </row>
     <row r="85">
@@ -1879,13 +1879,13 @@
         <v>50</v>
       </c>
       <c r="C85" t="n">
-        <v>422.5</v>
+        <v>238.5</v>
       </c>
       <c r="D85" t="n">
-        <v>422.5</v>
+        <v>80.75</v>
       </c>
       <c r="E85" t="n">
-        <v>422.5</v>
+        <v>579.25</v>
       </c>
     </row>
     <row r="86">
@@ -1896,13 +1896,13 @@
         <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>405</v>
+        <v>226</v>
       </c>
       <c r="D86" t="n">
-        <v>405</v>
+        <v>67.75</v>
       </c>
       <c r="E86" t="n">
-        <v>405</v>
+        <v>586.25</v>
       </c>
     </row>
     <row r="87">
@@ -1913,13 +1913,13 @@
         <v>10</v>
       </c>
       <c r="C87" t="n">
-        <v>404</v>
+        <v>218.5</v>
       </c>
       <c r="D87" t="n">
-        <v>404</v>
+        <v>59</v>
       </c>
       <c r="E87" t="n">
-        <v>404</v>
+        <v>551</v>
       </c>
     </row>
     <row r="88">
@@ -1930,13 +1930,13 @@
         <v>20</v>
       </c>
       <c r="C88" t="n">
-        <v>376</v>
+        <v>208</v>
       </c>
       <c r="D88" t="n">
-        <v>376</v>
+        <v>40.75</v>
       </c>
       <c r="E88" t="n">
-        <v>376</v>
+        <v>513.75</v>
       </c>
     </row>
     <row r="89">
@@ -1947,13 +1947,13 @@
         <v>30</v>
       </c>
       <c r="C89" t="n">
-        <v>370</v>
+        <v>173</v>
       </c>
       <c r="D89" t="n">
-        <v>370</v>
+        <v>29</v>
       </c>
       <c r="E89" t="n">
-        <v>370</v>
+        <v>503</v>
       </c>
     </row>
     <row r="90">
@@ -1964,13 +1964,13 @@
         <v>40</v>
       </c>
       <c r="C90" t="n">
-        <v>361</v>
+        <v>154</v>
       </c>
       <c r="D90" t="n">
-        <v>361</v>
+        <v>19</v>
       </c>
       <c r="E90" t="n">
-        <v>361</v>
+        <v>483</v>
       </c>
     </row>
     <row r="91">
@@ -1981,13 +1981,13 @@
         <v>50</v>
       </c>
       <c r="C91" t="n">
-        <v>344</v>
+        <v>144</v>
       </c>
       <c r="D91" t="n">
-        <v>344</v>
+        <v>14</v>
       </c>
       <c r="E91" t="n">
-        <v>344</v>
+        <v>453</v>
       </c>
     </row>
     <row r="92">
@@ -1998,13 +1998,13 @@
         <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>321.5</v>
+        <v>120</v>
       </c>
       <c r="D92" t="n">
-        <v>321.5</v>
+        <v>9.5</v>
       </c>
       <c r="E92" t="n">
-        <v>321.5</v>
+        <v>416.25</v>
       </c>
     </row>
     <row r="93">
@@ -2015,13 +2015,13 @@
         <v>10</v>
       </c>
       <c r="C93" t="n">
-        <v>310.5</v>
+        <v>97.5</v>
       </c>
       <c r="D93" t="n">
-        <v>310.5</v>
+        <v>6.025000095367432</v>
       </c>
       <c r="E93" t="n">
-        <v>310.5</v>
+        <v>373.5</v>
       </c>
     </row>
     <row r="94">
@@ -2032,13 +2032,13 @@
         <v>20</v>
       </c>
       <c r="C94" t="n">
-        <v>285</v>
+        <v>86</v>
       </c>
       <c r="D94" t="n">
-        <v>285</v>
+        <v>4.199999809265137</v>
       </c>
       <c r="E94" t="n">
-        <v>285</v>
+        <v>332</v>
       </c>
     </row>
     <row r="95">
@@ -2049,13 +2049,13 @@
         <v>30</v>
       </c>
       <c r="C95" t="n">
-        <v>273</v>
+        <v>69</v>
       </c>
       <c r="D95" t="n">
-        <v>273</v>
+        <v>3.5</v>
       </c>
       <c r="E95" t="n">
-        <v>273</v>
+        <v>321.75</v>
       </c>
     </row>
     <row r="96">
@@ -2066,13 +2066,13 @@
         <v>40</v>
       </c>
       <c r="C96" t="n">
-        <v>252.5</v>
+        <v>50.5</v>
       </c>
       <c r="D96" t="n">
-        <v>252.5</v>
+        <v>3.299999952316284</v>
       </c>
       <c r="E96" t="n">
-        <v>252.5</v>
+        <v>321.5</v>
       </c>
     </row>
     <row r="97">
@@ -2083,13 +2083,13 @@
         <v>50</v>
       </c>
       <c r="C97" t="n">
-        <v>235</v>
+        <v>38</v>
       </c>
       <c r="D97" t="n">
-        <v>235</v>
+        <v>3.099999904632568</v>
       </c>
       <c r="E97" t="n">
-        <v>235</v>
+        <v>285.75</v>
       </c>
     </row>
     <row r="98">
@@ -2100,13 +2100,13 @@
         <v>0</v>
       </c>
       <c r="C98" t="n">
-        <v>225.5</v>
+        <v>29.5</v>
       </c>
       <c r="D98" t="n">
-        <v>225.5</v>
+        <v>3.099999904632568</v>
       </c>
       <c r="E98" t="n">
-        <v>225.5</v>
+        <v>266</v>
       </c>
     </row>
     <row r="99">
@@ -2117,13 +2117,13 @@
         <v>10</v>
       </c>
       <c r="C99" t="n">
-        <v>211</v>
+        <v>17</v>
       </c>
       <c r="D99" t="n">
-        <v>211</v>
+        <v>3</v>
       </c>
       <c r="E99" t="n">
-        <v>211</v>
+        <v>239</v>
       </c>
     </row>
     <row r="100">
@@ -2134,13 +2134,13 @@
         <v>20</v>
       </c>
       <c r="C100" t="n">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="D100" t="n">
-        <v>199</v>
+        <v>3</v>
       </c>
       <c r="E100" t="n">
-        <v>199</v>
+        <v>213</v>
       </c>
     </row>
     <row r="101">
@@ -2151,13 +2151,13 @@
         <v>30</v>
       </c>
       <c r="C101" t="n">
-        <v>168</v>
+        <v>10</v>
       </c>
       <c r="D101" t="n">
-        <v>168</v>
+        <v>3</v>
       </c>
       <c r="E101" t="n">
-        <v>168</v>
+        <v>198</v>
       </c>
     </row>
     <row r="102">
@@ -2168,13 +2168,13 @@
         <v>40</v>
       </c>
       <c r="C102" t="n">
-        <v>151</v>
+        <v>5.699999809265137</v>
       </c>
       <c r="D102" t="n">
-        <v>151</v>
+        <v>2.900000095367432</v>
       </c>
       <c r="E102" t="n">
-        <v>151</v>
+        <v>174</v>
       </c>
     </row>
     <row r="103">
@@ -2185,13 +2185,13 @@
         <v>50</v>
       </c>
       <c r="C103" t="n">
-        <v>138.5</v>
+        <v>5.300000190734863</v>
       </c>
       <c r="D103" t="n">
-        <v>138.5</v>
+        <v>2.900000095367432</v>
       </c>
       <c r="E103" t="n">
-        <v>138.5</v>
+        <v>149.25</v>
       </c>
     </row>
     <row r="104">
@@ -2202,13 +2202,13 @@
         <v>0</v>
       </c>
       <c r="C104" t="n">
-        <v>120</v>
+        <v>4.75</v>
       </c>
       <c r="D104" t="n">
-        <v>120</v>
+        <v>2.900000095367432</v>
       </c>
       <c r="E104" t="n">
-        <v>120</v>
+        <v>139</v>
       </c>
     </row>
     <row r="105">
@@ -2219,13 +2219,13 @@
         <v>10</v>
       </c>
       <c r="C105" t="n">
-        <v>98</v>
+        <v>4.099999904632568</v>
       </c>
       <c r="D105" t="n">
-        <v>98</v>
+        <v>2.799999952316284</v>
       </c>
       <c r="E105" t="n">
-        <v>98</v>
+        <v>131</v>
       </c>
     </row>
     <row r="106">
@@ -2236,13 +2236,13 @@
         <v>20</v>
       </c>
       <c r="C106" t="n">
-        <v>86</v>
+        <v>3.900000095367432</v>
       </c>
       <c r="D106" t="n">
-        <v>86</v>
+        <v>2.799999952316284</v>
       </c>
       <c r="E106" t="n">
-        <v>86</v>
+        <v>108</v>
       </c>
     </row>
     <row r="107">
@@ -2253,13 +2253,13 @@
         <v>30</v>
       </c>
       <c r="C107" t="n">
-        <v>69</v>
+        <v>3.700000047683716</v>
       </c>
       <c r="D107" t="n">
-        <v>69</v>
+        <v>2.799999952316284</v>
       </c>
       <c r="E107" t="n">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
     <row r="108">
@@ -2270,13 +2270,13 @@
         <v>40</v>
       </c>
       <c r="C108" t="n">
-        <v>50</v>
+        <v>3.599999904632568</v>
       </c>
       <c r="D108" t="n">
-        <v>50</v>
+        <v>2.799999952316284</v>
       </c>
       <c r="E108" t="n">
-        <v>50</v>
+        <v>73</v>
       </c>
     </row>
     <row r="109">
@@ -2287,13 +2287,13 @@
         <v>50</v>
       </c>
       <c r="C109" t="n">
-        <v>38</v>
+        <v>3.599999904632568</v>
       </c>
       <c r="D109" t="n">
-        <v>38</v>
+        <v>2.799999952316284</v>
       </c>
       <c r="E109" t="n">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="110">
@@ -2304,13 +2304,13 @@
         <v>0</v>
       </c>
       <c r="C110" t="n">
-        <v>29</v>
+        <v>3.599999904632568</v>
       </c>
       <c r="D110" t="n">
-        <v>29</v>
+        <v>2.799999952316284</v>
       </c>
       <c r="E110" t="n">
-        <v>29</v>
+        <v>54</v>
       </c>
     </row>
     <row r="111">
@@ -2321,13 +2321,13 @@
         <v>10</v>
       </c>
       <c r="C111" t="n">
-        <v>17</v>
+        <v>3.5</v>
       </c>
       <c r="D111" t="n">
-        <v>17</v>
+        <v>2.799999952316284</v>
       </c>
       <c r="E111" t="n">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="112">
@@ -2338,13 +2338,13 @@
         <v>20</v>
       </c>
       <c r="C112" t="n">
-        <v>14</v>
+        <v>3.5</v>
       </c>
       <c r="D112" t="n">
-        <v>14</v>
+        <v>2.799999952316284</v>
       </c>
       <c r="E112" t="n">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="113">
@@ -2355,13 +2355,13 @@
         <v>30</v>
       </c>
       <c r="C113" t="n">
-        <v>10</v>
+        <v>3.5</v>
       </c>
       <c r="D113" t="n">
-        <v>10</v>
+        <v>2.799999952316284</v>
       </c>
       <c r="E113" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="114">
@@ -2372,13 +2372,13 @@
         <v>40</v>
       </c>
       <c r="C114" t="n">
-        <v>5.699999809265137</v>
+        <v>3.400000095367432</v>
       </c>
       <c r="D114" t="n">
-        <v>5.699999809265137</v>
+        <v>2.799999952316284</v>
       </c>
       <c r="E114" t="n">
-        <v>5.699999809265137</v>
+        <v>16</v>
       </c>
     </row>
     <row r="115">
@@ -2389,13 +2389,13 @@
         <v>50</v>
       </c>
       <c r="C115" t="n">
-        <v>5.300000190734863</v>
+        <v>3.400000095367432</v>
       </c>
       <c r="D115" t="n">
-        <v>5.300000190734863</v>
+        <v>2.799999952316284</v>
       </c>
       <c r="E115" t="n">
-        <v>5.300000190734863</v>
+        <v>13</v>
       </c>
     </row>
     <row r="116">
@@ -2406,13 +2406,13 @@
         <v>0</v>
       </c>
       <c r="C116" t="n">
-        <v>4.699999809265137</v>
+        <v>3.299999952316284</v>
       </c>
       <c r="D116" t="n">
-        <v>4.699999809265137</v>
+        <v>2.799999952316284</v>
       </c>
       <c r="E116" t="n">
-        <v>4.699999809265137</v>
+        <v>9.899999618530273</v>
       </c>
     </row>
     <row r="117">
@@ -2423,13 +2423,13 @@
         <v>10</v>
       </c>
       <c r="C117" t="n">
-        <v>4.099999904632568</v>
+        <v>3.299999952316284</v>
       </c>
       <c r="D117" t="n">
-        <v>4.099999904632568</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E117" t="n">
-        <v>4.099999904632568</v>
+        <v>6.699999809265137</v>
       </c>
     </row>
     <row r="118">
@@ -2440,13 +2440,13 @@
         <v>20</v>
       </c>
       <c r="C118" t="n">
-        <v>3.900000095367432</v>
+        <v>3.299999952316284</v>
       </c>
       <c r="D118" t="n">
-        <v>3.900000095367432</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E118" t="n">
-        <v>3.900000095367432</v>
+        <v>5.400000095367432</v>
       </c>
     </row>
     <row r="119">
@@ -2457,13 +2457,13 @@
         <v>30</v>
       </c>
       <c r="C119" t="n">
-        <v>3.700000047683716</v>
+        <v>3.299999952316284</v>
       </c>
       <c r="D119" t="n">
-        <v>3.700000047683716</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E119" t="n">
-        <v>3.700000047683716</v>
+        <v>4.800000190734863</v>
       </c>
     </row>
     <row r="120">
@@ -2474,13 +2474,13 @@
         <v>40</v>
       </c>
       <c r="C120" t="n">
-        <v>3.599999904632568</v>
+        <v>3.299999952316284</v>
       </c>
       <c r="D120" t="n">
-        <v>3.599999904632568</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E120" t="n">
-        <v>3.599999904632568</v>
+        <v>4.599999904632568</v>
       </c>
     </row>
     <row r="121">
@@ -2491,13 +2491,13 @@
         <v>50</v>
       </c>
       <c r="C121" t="n">
-        <v>3.599999904632568</v>
+        <v>3.299999952316284</v>
       </c>
       <c r="D121" t="n">
-        <v>3.599999904632568</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E121" t="n">
-        <v>3.599999904632568</v>
+        <v>4.400000095367432</v>
       </c>
     </row>
     <row r="122">
@@ -2508,13 +2508,13 @@
         <v>0</v>
       </c>
       <c r="C122" t="n">
-        <v>3.599999904632568</v>
+        <v>3.299999952316284</v>
       </c>
       <c r="D122" t="n">
-        <v>3.599999904632568</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E122" t="n">
-        <v>3.599999904632568</v>
+        <v>4.300000190734863</v>
       </c>
     </row>
     <row r="123">
@@ -2525,13 +2525,13 @@
         <v>10</v>
       </c>
       <c r="C123" t="n">
-        <v>3.5</v>
+        <v>3.200000047683716</v>
       </c>
       <c r="D123" t="n">
-        <v>3.5</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E123" t="n">
-        <v>3.5</v>
+        <v>4.199999809265137</v>
       </c>
     </row>
     <row r="124">
@@ -2542,13 +2542,13 @@
         <v>20</v>
       </c>
       <c r="C124" t="n">
-        <v>3.5</v>
+        <v>3.200000047683716</v>
       </c>
       <c r="D124" t="n">
-        <v>3.5</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E124" t="n">
-        <v>3.5</v>
+        <v>4.099999904632568</v>
       </c>
     </row>
     <row r="125">
@@ -2559,13 +2559,13 @@
         <v>30</v>
       </c>
       <c r="C125" t="n">
-        <v>3.5</v>
+        <v>3.200000047683716</v>
       </c>
       <c r="D125" t="n">
-        <v>3.5</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E125" t="n">
-        <v>3.5</v>
+        <v>4.099999904632568</v>
       </c>
     </row>
     <row r="126">
@@ -2576,13 +2576,13 @@
         <v>40</v>
       </c>
       <c r="C126" t="n">
-        <v>3.400000095367432</v>
+        <v>3.200000047683716</v>
       </c>
       <c r="D126" t="n">
-        <v>3.400000095367432</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E126" t="n">
-        <v>3.400000095367432</v>
+        <v>4.099999904632568</v>
       </c>
     </row>
     <row r="127">
@@ -2593,13 +2593,13 @@
         <v>50</v>
       </c>
       <c r="C127" t="n">
-        <v>3.400000095367432</v>
+        <v>3.200000047683716</v>
       </c>
       <c r="D127" t="n">
-        <v>3.400000095367432</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E127" t="n">
-        <v>3.400000095367432</v>
+        <v>4.099999904632568</v>
       </c>
     </row>
     <row r="128">
@@ -2610,13 +2610,13 @@
         <v>0</v>
       </c>
       <c r="C128" t="n">
-        <v>3.299999952316284</v>
+        <v>3.200000047683716</v>
       </c>
       <c r="D128" t="n">
-        <v>3.299999952316284</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E128" t="n">
-        <v>3.299999952316284</v>
+        <v>4.099999904632568</v>
       </c>
     </row>
     <row r="129">
@@ -2627,13 +2627,13 @@
         <v>10</v>
       </c>
       <c r="C129" t="n">
-        <v>3.299999952316284</v>
+        <v>3.200000047683716</v>
       </c>
       <c r="D129" t="n">
-        <v>3.299999952316284</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E129" t="n">
-        <v>3.299999952316284</v>
+        <v>4</v>
       </c>
     </row>
     <row r="130">
@@ -2644,13 +2644,13 @@
         <v>20</v>
       </c>
       <c r="C130" t="n">
-        <v>3.299999952316284</v>
+        <v>3.200000047683716</v>
       </c>
       <c r="D130" t="n">
-        <v>3.299999952316284</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E130" t="n">
-        <v>3.299999952316284</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131">
@@ -2661,13 +2661,13 @@
         <v>30</v>
       </c>
       <c r="C131" t="n">
-        <v>3.299999952316284</v>
+        <v>3.200000047683716</v>
       </c>
       <c r="D131" t="n">
-        <v>3.299999952316284</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E131" t="n">
-        <v>3.299999952316284</v>
+        <v>3.925000071525574</v>
       </c>
     </row>
     <row r="132">
@@ -2678,13 +2678,13 @@
         <v>40</v>
       </c>
       <c r="C132" t="n">
-        <v>3.299999952316284</v>
+        <v>3.200000047683716</v>
       </c>
       <c r="D132" t="n">
-        <v>3.299999952316284</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E132" t="n">
-        <v>3.299999952316284</v>
+        <v>4</v>
       </c>
     </row>
     <row r="133">
@@ -2695,13 +2695,13 @@
         <v>50</v>
       </c>
       <c r="C133" t="n">
-        <v>3.299999952316284</v>
+        <v>3.200000047683716</v>
       </c>
       <c r="D133" t="n">
-        <v>3.299999952316284</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E133" t="n">
-        <v>3.299999952316284</v>
+        <v>3.925000071525574</v>
       </c>
     </row>
     <row r="134">
@@ -2712,13 +2712,13 @@
         <v>0</v>
       </c>
       <c r="C134" t="n">
-        <v>3.299999952316284</v>
+        <v>3.200000047683716</v>
       </c>
       <c r="D134" t="n">
-        <v>3.299999952316284</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E134" t="n">
-        <v>3.299999952316284</v>
+        <v>3.900000095367432</v>
       </c>
     </row>
     <row r="135">
@@ -2729,13 +2729,13 @@
         <v>10</v>
       </c>
       <c r="C135" t="n">
-        <v>3.25</v>
+        <v>3.200000047683716</v>
       </c>
       <c r="D135" t="n">
-        <v>3.25</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E135" t="n">
-        <v>3.25</v>
+        <v>3.900000095367432</v>
       </c>
     </row>
     <row r="136">
@@ -2746,13 +2746,13 @@
         <v>20</v>
       </c>
       <c r="C136" t="n">
-        <v>3.25</v>
+        <v>3.200000047683716</v>
       </c>
       <c r="D136" t="n">
-        <v>3.25</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E136" t="n">
-        <v>3.25</v>
+        <v>3.900000095367432</v>
       </c>
     </row>
     <row r="137">
@@ -2766,10 +2766,10 @@
         <v>3.200000047683716</v>
       </c>
       <c r="D137" t="n">
-        <v>3.200000047683716</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E137" t="n">
-        <v>3.200000047683716</v>
+        <v>3.900000095367432</v>
       </c>
     </row>
     <row r="138">
@@ -2783,10 +2783,10 @@
         <v>3.200000047683716</v>
       </c>
       <c r="D138" t="n">
-        <v>3.200000047683716</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E138" t="n">
-        <v>3.200000047683716</v>
+        <v>3.900000095367432</v>
       </c>
     </row>
     <row r="139">
@@ -2800,10 +2800,10 @@
         <v>3.200000047683716</v>
       </c>
       <c r="D139" t="n">
-        <v>3.200000047683716</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E139" t="n">
-        <v>3.200000047683716</v>
+        <v>3.824999988079071</v>
       </c>
     </row>
     <row r="140">
@@ -2817,10 +2817,10 @@
         <v>3.200000047683716</v>
       </c>
       <c r="D140" t="n">
-        <v>3.200000047683716</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E140" t="n">
-        <v>3.200000047683716</v>
+        <v>3.799999952316284</v>
       </c>
     </row>
     <row r="141">
@@ -2834,10 +2834,10 @@
         <v>3.200000047683716</v>
       </c>
       <c r="D141" t="n">
-        <v>3.200000047683716</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E141" t="n">
-        <v>3.200000047683716</v>
+        <v>3.799999952316284</v>
       </c>
     </row>
     <row r="142">
@@ -2851,10 +2851,10 @@
         <v>3.200000047683716</v>
       </c>
       <c r="D142" t="n">
-        <v>3.200000047683716</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E142" t="n">
-        <v>3.200000047683716</v>
+        <v>3.799999952316284</v>
       </c>
     </row>
     <row r="143">
@@ -2868,10 +2868,10 @@
         <v>3.200000047683716</v>
       </c>
       <c r="D143" t="n">
-        <v>3.200000047683716</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E143" t="n">
-        <v>3.200000047683716</v>
+        <v>3.799999952316284</v>
       </c>
     </row>
     <row r="144">
@@ -2882,13 +2882,13 @@
         <v>40</v>
       </c>
       <c r="C144" t="n">
-        <v>3.200000047683716</v>
+        <v>3.099999904632568</v>
       </c>
       <c r="D144" t="n">
-        <v>3.200000047683716</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E144" t="n">
-        <v>3.200000047683716</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="145">
@@ -2899,13 +2899,13 @@
         <v>50</v>
       </c>
       <c r="C145" t="n">
-        <v>3.200000047683716</v>
+        <v>3.099999904632568</v>
       </c>
       <c r="D145" t="n">
-        <v>3.200000047683716</v>
+        <v>2.700000047683716</v>
       </c>
       <c r="E145" t="n">
-        <v>3.200000047683716</v>
+        <v>3.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>